<commit_message>
added initial commit of profile screen and Map API key issues in issue_traking_sheet.
</commit_message>
<xml_diff>
--- a/issue_tracking_sheet.xlsx
+++ b/issue_tracking_sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Issue Info</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Map API key not working for signed APK.</t>
+  </si>
+  <si>
+    <t>Inprogress</t>
   </si>
 </sst>
 </file>
@@ -63,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +384,7 @@
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -391,6 +399,17 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>